<commit_message>
Update project documentation and manuals for Sistema de Gestión de Horarios (SGH)
</commit_message>
<xml_diff>
--- a/Soportes/2.1.Ficha Tecnica.xlsx
+++ b/Soportes/2.1.Ficha Tecnica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Sebastian Gonza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Racinger\OneDrive\Escritorio\RepoSGH\SGH-docs\Soportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_84F4BB29F675A75B5846C095FC4A00DFAF2ED5FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB396BA2-71FC-46C9-94D9-5FFB2959C1B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDE9DEB-76A0-4255-A642-BACC9B231457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ficha Técnica de Software" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -99,9 +100,6 @@
     <t>LENGUAJES DE PROGRAMACIÓN</t>
   </si>
   <si>
-    <t>Frontend: React Native, React.Js, Css</t>
-  </si>
-  <si>
     <t>Backend: java (spring boot)</t>
   </si>
   <si>
@@ -123,9 +121,6 @@
     <t>IDEs : Visual Studio Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Base de datos: Xampp </t>
-  </si>
-  <si>
     <t>Control de versiones: Git, Github</t>
   </si>
   <si>
@@ -463,13 +458,19 @@
   </si>
   <si>
     <t>¿Se menciona el tipo de garantía que ofrece el hardware?</t>
+  </si>
+  <si>
+    <t>Frontend: React Native, Next.Js, Css</t>
+  </si>
+  <si>
+    <t>Base de datos: Mysql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -571,6 +572,21 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -853,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -865,9 +881,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -908,45 +921,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -959,59 +947,90 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,7 +1051,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1123,7 +1142,7 @@
                   <c:v>Mejorar la eficiencia en la gestión y control de los horarios para los docentes y estudiantes.</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Frontend: React Native, React.Js, Css</c:v>
+                  <c:v>Frontend: React Native, Next.Js, Css</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Backend: java (spring boot)</c:v>
@@ -1135,7 +1154,7 @@
                   <c:v>IDEs : Visual Studio Code</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Base de datos: Xampp </c:v>
+                  <c:v>Base de datos: Mysql</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>Control de versiones: Git, Github</c:v>
@@ -1321,7 +1340,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1329,6 +1347,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2149,29 +2168,29 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="59.109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:2" ht="12.75">
-      <c r="A2" s="56" t="s">
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2" ht="13.2">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-    </row>
-    <row r="3" spans="1:2" ht="12.75">
+      <c r="B2" s="32"/>
+    </row>
+    <row r="3" spans="1:2" ht="13.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2179,7 +2198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75">
+    <row r="4" spans="1:2" ht="13.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2187,7 +2206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75">
+    <row r="5" spans="1:2" ht="13.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2195,130 +2214,130 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:2" ht="13.2">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:2" ht="13.2">
+      <c r="A7" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75">
-      <c r="A8" s="42"/>
+    <row r="8" spans="1:2" ht="13.2">
+      <c r="A8" s="34"/>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.75">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:2" ht="13.2">
+      <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="36"/>
     </row>
     <row r="10" spans="1:2" ht="25.5" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:2" ht="26.4">
+      <c r="A11" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="65"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="69"/>
+      <c r="B14" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="21" t="s">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A15" s="70" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A16" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="46" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="32" t="s">
+      <c r="B17" s="66"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A18" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="33"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="34" t="s">
+      <c r="B18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="20" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A19" s="73"/>
+      <c r="B19" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A20" s="73"/>
+      <c r="B20" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="20" t="s">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21" s="74"/>
+      <c r="B21" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="35"/>
-      <c r="B20" s="20" t="s">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22" s="75" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="36"/>
-      <c r="B21" s="20" t="s">
+      <c r="B22" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" s="28" t="s">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -2337,8 +2356,8 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2366,399 +2385,393 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" ht="13.2">
+      <c r="A1" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
+    </row>
+    <row r="2" spans="1:7" ht="13.2">
+      <c r="A2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-    </row>
-    <row r="2" spans="1:7" ht="12.75">
-      <c r="A2" s="11" t="s">
+      <c r="C2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="3" spans="1:7" ht="13.2">
+      <c r="A3" s="41">
+        <v>2</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.75">
-      <c r="A3" s="48">
-        <v>2</v>
-      </c>
-      <c r="B3" s="48" t="s">
+      <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="13.2">
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="12.75">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="13.2">
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="12.75">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="13.2">
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.2">
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="12.75">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="56" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.75">
-      <c r="A7" s="60"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.2">
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.2">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="12.75">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="13.2">
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="13.2">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="13.2">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+    </row>
+    <row r="13" spans="1:7" ht="13.2">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.2">
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+    </row>
+    <row r="15" spans="1:7" ht="13.2">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="13.2">
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="13.2">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.2">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.2">
+      <c r="A19" s="41">
+        <v>1</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.2">
+      <c r="A20" s="44"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" ht="13.2">
+      <c r="A21" s="44"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="13.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="44"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="44"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="40" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="12.75">
-      <c r="A9" s="60"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D26" s="40"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="44"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="D27" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="44"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="12.75">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" ht="12.75">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.75">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-    </row>
-    <row r="13" spans="1:7" ht="12.75">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="D29" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D30" s="40"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31" s="44"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="12.75">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-    </row>
-    <row r="15" spans="1:7" ht="12.75">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="D31" s="23"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D32" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.75">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="1" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" s="44"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="12.75">
-      <c r="A17" s="60"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="3" t="s">
+      <c r="D33" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="3" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A34" s="45"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75">
-      <c r="A18" s="61"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.75">
-      <c r="A19" s="48">
-        <v>1</v>
-      </c>
-      <c r="B19" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75">
-      <c r="A20" s="53"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="1:5" ht="12.75">
-      <c r="A21" s="53"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75">
-      <c r="A22" s="53"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="22"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="53"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="53"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="53"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="22"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="53"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="53"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="53"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="53"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="52"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="53"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="53"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="54"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>33</v>
+      <c r="D34" s="26" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B34"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A3:A18"/>
-    <mergeCell ref="A19:A34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B3:B18"/>
@@ -2766,6 +2779,12 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="B19:B34"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A19:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2782,305 +2801,305 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="14.25">
-      <c r="A3" s="64" t="s">
+    <row r="3" spans="1:8" ht="13.8">
+      <c r="A3" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="13.2">
+      <c r="A4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="12.75">
-      <c r="A4" s="10" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.2">
+      <c r="A5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="12.75">
-      <c r="A5" s="10" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="13.2">
+      <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.75">
-      <c r="A6" s="10" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.2">
+      <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="12.75">
-      <c r="A7" s="10" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="13.2">
+      <c r="A8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="12.75">
-      <c r="A8" s="10" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.8">
+      <c r="A9" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="13.2">
+      <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.25">
-      <c r="A9" s="64" t="s">
+      <c r="B10" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="12.75">
-      <c r="A10" s="10" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="13.2">
+      <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="12.75">
-      <c r="A11" s="10" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="13.2">
+      <c r="A12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="12.75">
-      <c r="A12" s="10" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="13.8">
+      <c r="A13" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="13.2">
+      <c r="A14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.25">
-      <c r="A13" s="65" t="s">
+      <c r="B14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="12.75">
-      <c r="A14" s="10" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="13.2">
+      <c r="A15" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="12.75">
-      <c r="A15" s="10" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="13.2">
+      <c r="A16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.8">
+      <c r="A17" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="12.75">
-      <c r="A16" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="13.2">
+      <c r="A18" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="14.25">
-      <c r="A17" s="64" t="s">
+      <c r="B18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="12.75">
-      <c r="A18" s="10" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="13.2">
+      <c r="A19" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="12.75">
-      <c r="A19" s="10" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="13.8">
+      <c r="A20" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.2">
+      <c r="A21" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="14.25">
-      <c r="A20" s="65" t="s">
+      <c r="B21" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="12.75">
-      <c r="A21" s="10" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="13.2">
+      <c r="A22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="12.75">
-      <c r="A22" s="10" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="13.2">
+      <c r="A23" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="12.75">
-      <c r="A23" s="10" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="13.8">
+      <c r="A24" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="14.25">
-      <c r="A24" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="59"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="12.75">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
+    <row r="25" spans="1:6" ht="13.2">
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="12.75">
-      <c r="A26" s="69"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="70"/>
+    <row r="26" spans="1:6" ht="13.2">
+      <c r="A26" s="53"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="12.75">
-      <c r="A27" s="69"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="70"/>
+    <row r="27" spans="1:6" ht="13.2">
+      <c r="A27" s="53"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="12.75">
-      <c r="A28" s="69"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="70"/>
+    <row r="28" spans="1:6" ht="13.2">
+      <c r="A28" s="53"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="12.75">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="73"/>
+    <row r="29" spans="1:6" ht="13.2">
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3109,543 +3128,543 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="57.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="13.8">
+      <c r="A3" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="12"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+    </row>
+    <row r="4" spans="1:14" ht="13.2">
+      <c r="A4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.25">
-      <c r="A3" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="13"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-    </row>
-    <row r="4" spans="1:14" ht="12.75">
-      <c r="A4" s="16" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="12"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" ht="13.2">
+      <c r="A5" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="13"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" ht="12.75">
-      <c r="A5" s="16" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="12"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="1:14" ht="13.8">
+      <c r="A6" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="12"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" ht="13.2">
+      <c r="A7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="13"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.25">
-      <c r="A6" s="74" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="12"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="1:14" ht="13.2">
+      <c r="A8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="13"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-    </row>
-    <row r="7" spans="1:14" ht="12.75">
-      <c r="A7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="12"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="1:14" ht="13.2">
+      <c r="A9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="13"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" ht="12.75">
-      <c r="A8" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="16" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="12"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+    </row>
+    <row r="10" spans="1:14" ht="13.2">
+      <c r="A10" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="13"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" ht="12.75">
-      <c r="A9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="13"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" ht="12.75">
-      <c r="A10" s="16" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="12"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+    </row>
+    <row r="11" spans="1:14" ht="13.2">
+      <c r="A11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="12"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+    </row>
+    <row r="12" spans="1:14" ht="13.2">
+      <c r="A12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="13"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" ht="12.75">
-      <c r="A11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="12"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+    </row>
+    <row r="13" spans="1:14" ht="13.2">
+      <c r="A13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="13"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" ht="12.75">
-      <c r="A12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="12"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+    </row>
+    <row r="14" spans="1:14" ht="13.2">
+      <c r="A14" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="13"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" ht="12.75">
-      <c r="A13" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="13"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-    </row>
-    <row r="14" spans="1:14" ht="12.75">
-      <c r="A14" s="16" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="12"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:14" ht="13.2">
+      <c r="A15" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="13"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75">
-      <c r="A15" s="16" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="12"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:14" ht="13.2">
+      <c r="A16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="12"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="1:14" ht="13.2">
+      <c r="A17" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="13"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75">
-      <c r="A16" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="12"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="1:14" ht="13.2">
+      <c r="A18" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="13"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" ht="12.75">
-      <c r="A17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="13"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" ht="12.75">
-      <c r="A18" s="16" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="12"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:14" ht="13.2">
+      <c r="A19" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="13"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" ht="12.75">
-      <c r="A19" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="13"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" ht="14.25">
-      <c r="A20" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="13"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" ht="12.75">
-      <c r="A21" s="66"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="13"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" ht="12.75">
-      <c r="A22" s="69"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="13"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" ht="12.75">
-      <c r="A23" s="69"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="13"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-    </row>
-    <row r="24" spans="1:14" ht="12.75">
-      <c r="A24" s="69"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="13"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-    </row>
-    <row r="25" spans="1:14" ht="12.75">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="13"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-    </row>
-    <row r="26" spans="1:14" ht="12.75">
-      <c r="E26" s="13"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-    </row>
-    <row r="27" spans="1:14" ht="12.75">
-      <c r="E27" s="13"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-    </row>
-    <row r="28" spans="1:14" ht="12.75">
-      <c r="E28" s="13"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-    </row>
-    <row r="29" spans="1:14" ht="12.75">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-    </row>
-    <row r="30" spans="1:14" ht="12.75">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="13"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-    </row>
-    <row r="31" spans="1:14" ht="12.75">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="13"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-    </row>
-    <row r="32" spans="1:14" ht="12.75">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="13"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-    </row>
-    <row r="33" spans="1:14" ht="12.75">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="13"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" ht="12.75">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="13"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-    </row>
-    <row r="35" spans="1:14" ht="12.75">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="13"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-    </row>
-    <row r="36" spans="1:14" ht="12.75">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-    </row>
-    <row r="37" spans="1:14" ht="12.75">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:14" ht="12.75">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:14" ht="12.75">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:14" ht="12.75">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:14" ht="12.75">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:14" ht="12.75">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:14" ht="12.75">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="1:14" ht="12.75">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="1:14" ht="12.75">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="1:14" ht="12.75">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="1:14" ht="12.75">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="12"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" ht="13.8">
+      <c r="A20" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="12"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:14" ht="13.2">
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="12"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:14" ht="13.2">
+      <c r="A22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="12"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+    </row>
+    <row r="23" spans="1:14" ht="13.2">
+      <c r="A23" s="53"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="12"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+    </row>
+    <row r="24" spans="1:14" ht="13.2">
+      <c r="A24" s="53"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="12"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+    </row>
+    <row r="25" spans="1:14" ht="13.2">
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="12"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+    </row>
+    <row r="26" spans="1:14" ht="13.2">
+      <c r="E26" s="12"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="1:14" ht="13.2">
+      <c r="E27" s="12"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="1:14" ht="13.2">
+      <c r="E28" s="12"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+    </row>
+    <row r="29" spans="1:14" ht="13.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="12"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+    </row>
+    <row r="30" spans="1:14" ht="13.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+    </row>
+    <row r="31" spans="1:14" ht="13.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="12"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" ht="13.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="12"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+    </row>
+    <row r="33" spans="1:14" ht="13.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="12"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+    </row>
+    <row r="34" spans="1:14" ht="13.2">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="12"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+    </row>
+    <row r="35" spans="1:14" ht="13.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="12"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+    </row>
+    <row r="36" spans="1:14" ht="13.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14" ht="13.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:14" ht="13.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:14" ht="13.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:14" ht="13.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:14" ht="13.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="1:14" ht="13.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:14" ht="13.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" ht="13.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="1:14" ht="13.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:14" ht="13.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" ht="13.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3661,6 +3680,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8e4e03e1-f8b1-44af-8a18-d6c17e30f4d4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3f02ce4-f17e-46f8-88f7-72120ec08e56">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029D82C79E9C45A4F8892A5168669910F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ea8e158fdb56c00ff9dbd260d4d852a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3f02ce4-f17e-46f8-88f7-72120ec08e56" xmlns:ns3="8e4e03e1-f8b1-44af-8a18-d6c17e30f4d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfc354b75f42f41b3089271a87c970f8" ns2:_="" ns3:_="">
     <xsd:import namespace="e3f02ce4-f17e-46f8-88f7-72120ec08e56"/>
@@ -3861,34 +3900,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8e4e03e1-f8b1-44af-8a18-d6c17e30f4d4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3f02ce4-f17e-46f8-88f7-72120ec08e56">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E71FACC8-7D8F-46B7-8179-17820579DFE1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EBA8E9-E25E-4879-B9AD-8BC911D5F6B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875EC937-74AF-4AB4-AC43-E07AACF6CC1D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875EC937-74AF-4AB4-AC43-E07AACF6CC1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e4e03e1-f8b1-44af-8a18-d6c17e30f4d4"/>
+    <ds:schemaRef ds:uri="e3f02ce4-f17e-46f8-88f7-72120ec08e56"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EBA8E9-E25E-4879-B9AD-8BC911D5F6B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E71FACC8-7D8F-46B7-8179-17820579DFE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e3f02ce4-f17e-46f8-88f7-72120ec08e56"/>
+    <ds:schemaRef ds:uri="8e4e03e1-f8b1-44af-8a18-d6c17e30f4d4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>